<commit_message>
typo and changing Fungal sp. to Fungus
</commit_message>
<xml_diff>
--- a/Data/TABLE_S3_COM3.xlsx
+++ b/Data/TABLE_S3_COM3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909462B3-065E-43F9-A3A1-F4FDCE7E18A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CED753-2EA3-45EE-9939-B25C868196D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -916,9 +916,6 @@
     <t>PP110784, NR_163686, NR_136117, NR_135927</t>
   </si>
   <si>
-    <t xml:space="preserve">Fungal sp. </t>
-  </si>
-  <si>
     <t>KY102355 type</t>
   </si>
   <si>
@@ -4413,6 +4410,9 @@
   </si>
   <si>
     <t>Subphylum; order; family (after Mycobank)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fungus sp. </t>
   </si>
 </sst>
 </file>
@@ -4656,6 +4656,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4663,9 +4666,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5465,8 +5465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L141" sqref="L141"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
@@ -5483,48 +5483,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="52.95" customHeight="1">
-      <c r="A1" s="24" t="s">
-        <v>562</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
+      <c r="A1" s="25" t="s">
+        <v>561</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="99" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>414</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>309</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>310</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>0</v>
@@ -5532,13 +5532,13 @@
       <c r="K2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="27" t="s">
-        <v>609</v>
+      <c r="L2" s="24" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16.95" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B3" s="6">
         <v>3</v>
@@ -5559,7 +5559,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>295</v>
@@ -5571,12 +5571,12 @@
         <v>100</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="16.2" customHeight="1">
       <c r="A4" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C4" s="12">
         <v>1</v>
@@ -5588,10 +5588,10 @@
         <v>5</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J4" s="16">
         <v>100</v>
@@ -5600,7 +5600,7 @@
         <v>100</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -5617,7 +5617,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>10</v>
@@ -5629,12 +5629,12 @@
         <v>100</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="6">
@@ -5647,10 +5647,10 @@
         <v>12</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J6" s="16">
         <v>100</v>
@@ -5659,12 +5659,12 @@
         <v>100</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="6">
@@ -5677,10 +5677,10 @@
         <v>11</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I7" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J7" s="16">
         <v>100</v>
@@ -5689,7 +5689,7 @@
         <v>100</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5712,7 +5712,7 @@
         <v>13</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I8" s="19" t="s">
         <v>14</v>
@@ -5724,12 +5724,12 @@
         <v>75</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B9" s="6">
         <v>2</v>
@@ -5742,7 +5742,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>18</v>
@@ -5754,7 +5754,7 @@
         <v>100</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5772,7 +5772,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>16</v>
@@ -5784,12 +5784,12 @@
         <v>100</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="6">
@@ -5802,7 +5802,7 @@
         <v>19</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I11" s="19" t="s">
         <v>20</v>
@@ -5814,12 +5814,12 @@
         <v>100</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="16" customFormat="1">
       <c r="A12" s="20" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
@@ -5834,10 +5834,10 @@
         <v>4</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J12" s="16">
         <v>100</v>
@@ -5846,12 +5846,12 @@
         <v>100</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="6">
@@ -5867,7 +5867,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>22</v>
@@ -5879,12 +5879,12 @@
         <v>100</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="6">
@@ -5897,7 +5897,7 @@
         <v>23</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>24</v>
@@ -5909,7 +5909,7 @@
         <v>100</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -5927,7 +5927,7 @@
         <v>25</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>26</v>
@@ -5939,12 +5939,12 @@
         <v>100</v>
       </c>
       <c r="L15" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="18" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B16" s="6">
         <v>1</v>
@@ -5965,7 +5965,7 @@
         <v>29</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>30</v>
@@ -5977,12 +5977,12 @@
         <v>100</v>
       </c>
       <c r="L16" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="34.950000000000003" customHeight="1">
       <c r="A17" s="16" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C17" s="12">
         <v>1</v>
@@ -5994,10 +5994,10 @@
         <v>28</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J17" s="16">
         <v>100</v>
@@ -6006,12 +6006,12 @@
         <v>100</v>
       </c>
       <c r="L17" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="34.200000000000003" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C18" s="12">
         <v>2</v>
@@ -6026,10 +6026,10 @@
         <v>27</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J18" s="16">
         <v>100</v>
@@ -6038,12 +6038,12 @@
         <v>100</v>
       </c>
       <c r="L18" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
@@ -6056,7 +6056,7 @@
         <v>31</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>32</v>
@@ -6068,7 +6068,7 @@
         <v>100</v>
       </c>
       <c r="L19" s="23" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -6088,10 +6088,10 @@
         <v>33</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J20" s="16">
         <v>100</v>
@@ -6100,7 +6100,7 @@
         <v>100</v>
       </c>
       <c r="L20" s="23" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -6117,7 +6117,7 @@
         <v>34</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I21" s="19" t="s">
         <v>35</v>
@@ -6129,12 +6129,12 @@
         <v>100</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B22" s="6">
         <v>1</v>
@@ -6147,10 +6147,10 @@
         <v>38</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J22" s="16">
         <v>100</v>
@@ -6159,12 +6159,12 @@
         <v>100</v>
       </c>
       <c r="L22" s="23" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B23" s="6">
         <v>1</v>
@@ -6177,7 +6177,7 @@
         <v>36</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>37</v>
@@ -6189,7 +6189,7 @@
         <v>100</v>
       </c>
       <c r="L23" s="23" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -6207,10 +6207,10 @@
         <v>39</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J24" s="16">
         <v>100</v>
@@ -6219,7 +6219,7 @@
         <v>100</v>
       </c>
       <c r="L24" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="16" customFormat="1">
@@ -6239,7 +6239,7 @@
         <v>40</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I25" s="19" t="s">
         <v>41</v>
@@ -6251,7 +6251,7 @@
         <v>100</v>
       </c>
       <c r="L25" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -6268,7 +6268,7 @@
         <v>43</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I26" s="19" t="s">
         <v>44</v>
@@ -6280,12 +6280,12 @@
         <v>100</v>
       </c>
       <c r="L26" s="23" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C27" s="12">
         <v>4</v>
@@ -6300,10 +6300,10 @@
         <v>42</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J27" s="16">
         <v>100</v>
@@ -6312,12 +6312,12 @@
         <v>100</v>
       </c>
       <c r="L27" s="23" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="16.95" customHeight="1">
       <c r="A28" s="16" t="s">
-        <v>296</v>
+        <v>609</v>
       </c>
       <c r="C28" s="12">
         <v>7</v>
@@ -6331,18 +6331,18 @@
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I28" s="19"/>
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
       <c r="L28" s="23" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="16.95" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="6">
@@ -6355,10 +6355,10 @@
         <v>48</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J29" s="16">
         <v>100</v>
@@ -6367,12 +6367,12 @@
         <v>100</v>
       </c>
       <c r="L29" s="23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="34.200000000000003" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C30" s="12">
         <v>1</v>
@@ -6384,10 +6384,10 @@
         <v>45</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J30" s="16">
         <v>100</v>
@@ -6396,7 +6396,7 @@
         <v>100</v>
       </c>
       <c r="L30" s="23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -6413,7 +6413,7 @@
         <v>46</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I31" s="19" t="s">
         <v>47</v>
@@ -6425,12 +6425,12 @@
         <v>100</v>
       </c>
       <c r="L31" s="23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="6">
@@ -6446,7 +6446,7 @@
         <v>52</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I32" s="19" t="s">
         <v>53</v>
@@ -6458,12 +6458,12 @@
         <v>100</v>
       </c>
       <c r="L32" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="6">
@@ -6476,7 +6476,7 @@
         <v>54</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I33" s="19" t="s">
         <v>55</v>
@@ -6488,12 +6488,12 @@
         <v>100</v>
       </c>
       <c r="L33" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C34" s="12">
         <v>1</v>
@@ -6508,7 +6508,7 @@
         <v>56</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I34" s="19" t="s">
         <v>57</v>
@@ -6520,12 +6520,12 @@
         <v>100</v>
       </c>
       <c r="L34" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C35" s="11"/>
       <c r="E35" s="6">
@@ -6538,7 +6538,7 @@
         <v>58</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I35" s="19" t="s">
         <v>59</v>
@@ -6550,12 +6550,12 @@
         <v>100</v>
       </c>
       <c r="L35" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" s="16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="6">
@@ -6571,7 +6571,7 @@
         <v>51</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I36" s="19" t="s">
         <v>50</v>
@@ -6583,12 +6583,12 @@
         <v>100</v>
       </c>
       <c r="L36" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37" s="16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="6">
@@ -6604,7 +6604,7 @@
         <v>49</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I37" s="19" t="s">
         <v>50</v>
@@ -6616,12 +6616,12 @@
         <v>100</v>
       </c>
       <c r="L37" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C38" s="12">
         <v>6</v>
@@ -6639,7 +6639,7 @@
         <v>60</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I38" s="19" t="s">
         <v>61</v>
@@ -6651,12 +6651,12 @@
         <v>100</v>
       </c>
       <c r="L38" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C39" s="12">
         <v>2</v>
@@ -6668,7 +6668,7 @@
         <v>62</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I39" s="19" t="s">
         <v>61</v>
@@ -6680,12 +6680,12 @@
         <v>100</v>
       </c>
       <c r="L39" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="16" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C40" s="12">
         <v>4</v>
@@ -6700,7 +6700,7 @@
         <v>63</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I40" s="19" t="s">
         <v>61</v>
@@ -6712,12 +6712,12 @@
         <v>100</v>
       </c>
       <c r="L40" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="16" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C41" s="12">
         <v>13</v>
@@ -6735,7 +6735,7 @@
         <v>64</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I41" s="19" t="s">
         <v>61</v>
@@ -6747,12 +6747,12 @@
         <v>100</v>
       </c>
       <c r="L41" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C42" s="12">
         <v>1</v>
@@ -6770,7 +6770,7 @@
         <v>65</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I42" s="19" t="s">
         <v>61</v>
@@ -6782,12 +6782,12 @@
         <v>100</v>
       </c>
       <c r="L42" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="16" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C43" s="12">
         <v>6</v>
@@ -6805,7 +6805,7 @@
         <v>66</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I43" s="19" t="s">
         <v>61</v>
@@ -6817,12 +6817,12 @@
         <v>100</v>
       </c>
       <c r="L43" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C44" s="12">
         <v>2</v>
@@ -6840,7 +6840,7 @@
         <v>67</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I44" s="19" t="s">
         <v>61</v>
@@ -6852,12 +6852,12 @@
         <v>100</v>
       </c>
       <c r="L44" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="16" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C45" s="12">
         <v>9</v>
@@ -6875,7 +6875,7 @@
         <v>68</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I45" s="19" t="s">
         <v>61</v>
@@ -6887,12 +6887,12 @@
         <v>100</v>
       </c>
       <c r="L45" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C46" s="11"/>
       <c r="E46" s="6">
@@ -6905,7 +6905,7 @@
         <v>69</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I46" s="19" t="s">
         <v>61</v>
@@ -6917,12 +6917,12 @@
         <v>100</v>
       </c>
       <c r="L46" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="6">
@@ -6935,7 +6935,7 @@
         <v>70</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I47" s="19" t="s">
         <v>61</v>
@@ -6947,12 +6947,12 @@
         <v>100</v>
       </c>
       <c r="L47" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C48" s="12">
         <v>2</v>
@@ -6970,7 +6970,7 @@
         <v>71</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I48" s="19" t="s">
         <v>61</v>
@@ -6982,12 +6982,12 @@
         <v>100</v>
       </c>
       <c r="L48" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="16" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="6">
@@ -7003,7 +7003,7 @@
         <v>72</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I49" s="19" t="s">
         <v>61</v>
@@ -7015,12 +7015,12 @@
         <v>100</v>
       </c>
       <c r="L49" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="6">
@@ -7033,7 +7033,7 @@
         <v>73</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I50" s="19" t="s">
         <v>61</v>
@@ -7045,12 +7045,12 @@
         <v>100</v>
       </c>
       <c r="L50" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C51" s="12">
         <v>4</v>
@@ -7068,7 +7068,7 @@
         <v>74</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I51" s="19" t="s">
         <v>61</v>
@@ -7080,12 +7080,12 @@
         <v>100</v>
       </c>
       <c r="L51" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="6">
@@ -7101,7 +7101,7 @@
         <v>75</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I52" s="19" t="s">
         <v>61</v>
@@ -7113,12 +7113,12 @@
         <v>100</v>
       </c>
       <c r="L52" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="6">
@@ -7131,7 +7131,7 @@
         <v>76</v>
       </c>
       <c r="H53" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I53" s="19" t="s">
         <v>61</v>
@@ -7143,12 +7143,12 @@
         <v>100</v>
       </c>
       <c r="L53" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="6">
@@ -7161,7 +7161,7 @@
         <v>77</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I54" s="19" t="s">
         <v>61</v>
@@ -7173,12 +7173,12 @@
         <v>100</v>
       </c>
       <c r="L54" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C55" s="11"/>
       <c r="E55" s="6">
@@ -7191,7 +7191,7 @@
         <v>78</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I55" s="19" t="s">
         <v>61</v>
@@ -7203,12 +7203,12 @@
         <v>96</v>
       </c>
       <c r="L55" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B56" s="6">
         <v>1</v>
@@ -7221,7 +7221,7 @@
         <v>79</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I56" s="19" t="s">
         <v>80</v>
@@ -7233,7 +7233,7 @@
         <v>100</v>
       </c>
       <c r="L56" s="23" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -7253,7 +7253,7 @@
         <v>81</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I57" s="19" t="s">
         <v>82</v>
@@ -7265,25 +7265,25 @@
         <v>100</v>
       </c>
       <c r="L57" s="23" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B58" s="6">
         <v>2</v>
       </c>
       <c r="C58" s="11"/>
       <c r="F58" s="16" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G58" s="16" t="s">
         <v>7</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I58" s="19" t="s">
         <v>8</v>
@@ -7295,12 +7295,12 @@
         <v>100</v>
       </c>
       <c r="L58" s="23" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="16" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C59" s="11"/>
       <c r="E59" s="6">
@@ -7313,7 +7313,7 @@
         <v>83</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I59" s="19" t="s">
         <v>84</v>
@@ -7325,12 +7325,12 @@
         <v>100</v>
       </c>
       <c r="L59" s="23" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="16" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C60" s="12">
         <v>1</v>
@@ -7340,13 +7340,13 @@
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>97</v>
       </c>
       <c r="H60" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I60" s="19" t="s">
         <v>98</v>
@@ -7358,12 +7358,12 @@
         <v>100</v>
       </c>
       <c r="L60" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="16" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="6">
@@ -7371,13 +7371,13 @@
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>99</v>
       </c>
       <c r="H61" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I61" s="19" t="s">
         <v>98</v>
@@ -7389,12 +7389,12 @@
         <v>100</v>
       </c>
       <c r="L61" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="6">
@@ -7408,7 +7408,7 @@
         <v>85</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I62" s="19" t="s">
         <v>86</v>
@@ -7420,12 +7420,12 @@
         <v>97</v>
       </c>
       <c r="L62" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C63" s="12">
         <v>1</v>
@@ -7438,7 +7438,7 @@
         <v>102</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I63" s="19" t="s">
         <v>95</v>
@@ -7450,12 +7450,12 @@
         <v>99</v>
       </c>
       <c r="L63" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="16" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C64" s="12">
         <v>3</v>
@@ -7471,7 +7471,7 @@
         <v>94</v>
       </c>
       <c r="H64" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I64" s="19" t="s">
         <v>95</v>
@@ -7483,12 +7483,12 @@
         <v>98</v>
       </c>
       <c r="L64" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="16" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C65" s="12">
         <v>2</v>
@@ -7501,7 +7501,7 @@
         <v>87</v>
       </c>
       <c r="H65" s="17" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I65" s="19" t="s">
         <v>88</v>
@@ -7513,12 +7513,12 @@
         <v>98</v>
       </c>
       <c r="L65" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C66" s="12">
         <v>10</v>
@@ -7534,7 +7534,7 @@
         <v>89</v>
       </c>
       <c r="H66" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I66" s="19" t="s">
         <v>88</v>
@@ -7546,12 +7546,12 @@
         <v>98</v>
       </c>
       <c r="L66" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C67" s="12">
         <v>1</v>
@@ -7567,7 +7567,7 @@
         <v>96</v>
       </c>
       <c r="H67" s="17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I67" s="19" t="s">
         <v>88</v>
@@ -7579,12 +7579,12 @@
         <v>98</v>
       </c>
       <c r="L67" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C68" s="12">
         <v>2</v>
@@ -7600,7 +7600,7 @@
         <v>100</v>
       </c>
       <c r="H68" s="17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I68" s="19" t="s">
         <v>88</v>
@@ -7612,12 +7612,12 @@
         <v>98</v>
       </c>
       <c r="L68" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="16" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C69" s="12">
         <v>1</v>
@@ -7630,7 +7630,7 @@
         <v>90</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I69" s="19" t="s">
         <v>91</v>
@@ -7642,12 +7642,12 @@
         <v>98</v>
       </c>
       <c r="L69" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="16" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C70" s="12">
         <v>2</v>
@@ -7663,7 +7663,7 @@
         <v>92</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I70" s="19" t="s">
         <v>93</v>
@@ -7675,12 +7675,12 @@
         <v>98</v>
       </c>
       <c r="L70" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="6">
@@ -7694,7 +7694,7 @@
         <v>101</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I71" s="19" t="s">
         <v>93</v>
@@ -7706,7 +7706,7 @@
         <v>100</v>
       </c>
       <c r="L71" s="23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -7727,7 +7727,7 @@
         <v>103</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I72" s="19" t="s">
         <v>104</v>
@@ -7739,12 +7739,12 @@
         <v>100</v>
       </c>
       <c r="L72" s="23" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="16" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C73" s="13"/>
       <c r="D73" s="6">
@@ -7760,7 +7760,7 @@
         <v>107</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I73" s="19" t="s">
         <v>108</v>
@@ -7772,12 +7772,12 @@
         <v>100</v>
       </c>
       <c r="L73" s="23" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="6">
@@ -7793,7 +7793,7 @@
         <v>105</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I74" s="19" t="s">
         <v>106</v>
@@ -7805,7 +7805,7 @@
         <v>100</v>
       </c>
       <c r="L74" s="23" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -7823,7 +7823,7 @@
         <v>109</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I75" s="19" t="s">
         <v>110</v>
@@ -7835,7 +7835,7 @@
         <v>100</v>
       </c>
       <c r="L75" s="23" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -7853,7 +7853,7 @@
         <v>111</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I76" s="19" t="s">
         <v>112</v>
@@ -7865,7 +7865,7 @@
         <v>100</v>
       </c>
       <c r="L76" s="23" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -7883,7 +7883,7 @@
         <v>115</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I77" s="19" t="s">
         <v>116</v>
@@ -7895,12 +7895,12 @@
         <v>100</v>
       </c>
       <c r="L77" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="16" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B78" s="8">
         <v>1</v>
@@ -7915,13 +7915,13 @@
         <v>4</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G78" s="16" t="s">
         <v>118</v>
       </c>
       <c r="H78" s="17" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I78" s="19" t="s">
         <v>119</v>
@@ -7933,7 +7933,7 @@
         <v>100</v>
       </c>
       <c r="L78" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -7950,7 +7950,7 @@
         <v>120</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I79" s="19" t="s">
         <v>121</v>
@@ -7962,7 +7962,7 @@
         <v>100</v>
       </c>
       <c r="L79" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -7980,7 +7980,7 @@
         <v>122</v>
       </c>
       <c r="H80" s="17" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I80" s="19" t="s">
         <v>123</v>
@@ -7992,12 +7992,12 @@
         <v>100</v>
       </c>
       <c r="L80" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="81" spans="1:40" ht="31.2">
       <c r="A81" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="6">
@@ -8013,10 +8013,10 @@
         <v>117</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I81" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J81" s="16">
         <v>100</v>
@@ -8025,12 +8025,12 @@
         <v>100</v>
       </c>
       <c r="L81" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="82" spans="1:40">
       <c r="A82" s="16" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C82" s="12">
         <v>1</v>
@@ -8042,7 +8042,7 @@
         <v>124</v>
       </c>
       <c r="H82" s="17" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I82" s="19" t="s">
         <v>125</v>
@@ -8054,12 +8054,12 @@
         <v>100</v>
       </c>
       <c r="L82" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="83" spans="1:40">
       <c r="A83" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B83" s="6">
         <v>1</v>
@@ -8072,10 +8072,10 @@
         <v>113</v>
       </c>
       <c r="H83" s="17" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J83" s="16">
         <v>100</v>
@@ -8084,7 +8084,7 @@
         <v>114</v>
       </c>
       <c r="L83" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="84" spans="1:40">
@@ -8096,13 +8096,13 @@
         <v>1</v>
       </c>
       <c r="F84" s="16" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G84" s="16" t="s">
         <v>126</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I84" s="19" t="s">
         <v>127</v>
@@ -8114,12 +8114,12 @@
         <v>100</v>
       </c>
       <c r="L84" s="23" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="85" spans="1:40" s="14" customFormat="1">
       <c r="A85" s="20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="11"/>
@@ -8130,13 +8130,13 @@
         <v>3</v>
       </c>
       <c r="F85" s="16" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G85" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H85" s="17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I85" s="19" t="s">
         <v>3</v>
@@ -8148,7 +8148,7 @@
         <v>100</v>
       </c>
       <c r="L85" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="M85" s="16"/>
       <c r="N85" s="16"/>
@@ -8181,7 +8181,7 @@
     </row>
     <row r="86" spans="1:40">
       <c r="A86" s="16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="6">
@@ -8197,7 +8197,7 @@
         <v>174</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I86" s="19" t="s">
         <v>175</v>
@@ -8209,7 +8209,7 @@
         <v>100</v>
       </c>
       <c r="L86" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="87" spans="1:40">
@@ -8232,7 +8232,7 @@
         <v>162</v>
       </c>
       <c r="H87" s="17" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I87" s="19" t="s">
         <v>163</v>
@@ -8244,12 +8244,12 @@
         <v>100</v>
       </c>
       <c r="L87" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="88" spans="1:40">
       <c r="A88" s="16" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="6">
@@ -8262,7 +8262,7 @@
         <v>154</v>
       </c>
       <c r="H88" s="17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I88" s="19" t="s">
         <v>155</v>
@@ -8274,12 +8274,12 @@
         <v>100</v>
       </c>
       <c r="L88" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="89" spans="1:40">
       <c r="A89" s="16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C89" s="12">
         <v>3</v>
@@ -8297,7 +8297,7 @@
         <v>173</v>
       </c>
       <c r="H89" s="17" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I89" s="19" t="s">
         <v>163</v>
@@ -8309,7 +8309,7 @@
         <v>100</v>
       </c>
       <c r="L89" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="90" spans="1:40">
@@ -8332,7 +8332,7 @@
         <v>166</v>
       </c>
       <c r="H90" s="17" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I90" s="19" t="s">
         <v>165</v>
@@ -8344,12 +8344,12 @@
         <v>95</v>
       </c>
       <c r="L90" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="91" spans="1:40">
       <c r="A91" s="16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C91" s="12">
         <v>5</v>
@@ -8367,7 +8367,7 @@
         <v>164</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I91" s="19" t="s">
         <v>165</v>
@@ -8379,12 +8379,12 @@
         <v>95</v>
       </c>
       <c r="L91" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="92" spans="1:40">
       <c r="A92" s="16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C92" s="11"/>
       <c r="E92" s="6">
@@ -8397,7 +8397,7 @@
         <v>167</v>
       </c>
       <c r="H92" s="17" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I92" s="19" t="s">
         <v>165</v>
@@ -8409,12 +8409,12 @@
         <v>95</v>
       </c>
       <c r="L92" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="93" spans="1:40">
       <c r="A93" s="16" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C93" s="12">
         <v>1</v>
@@ -8426,7 +8426,7 @@
         <v>168</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I93" s="19" t="s">
         <v>165</v>
@@ -8438,12 +8438,12 @@
         <v>95</v>
       </c>
       <c r="L93" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="94" spans="1:40">
       <c r="A94" s="16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C94" s="11"/>
       <c r="E94" s="6">
@@ -8456,7 +8456,7 @@
         <v>169</v>
       </c>
       <c r="H94" s="17" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I94" s="19" t="s">
         <v>165</v>
@@ -8468,12 +8468,12 @@
         <v>95</v>
       </c>
       <c r="L94" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="95" spans="1:40">
       <c r="A95" s="16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="6">
@@ -8486,7 +8486,7 @@
         <v>170</v>
       </c>
       <c r="H95" s="17" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I95" s="19" t="s">
         <v>165</v>
@@ -8498,12 +8498,12 @@
         <v>95</v>
       </c>
       <c r="L95" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="96" spans="1:40">
       <c r="A96" s="16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C96" s="10"/>
       <c r="D96" s="6">
@@ -8519,7 +8519,7 @@
         <v>147</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I96" s="19" t="s">
         <v>148</v>
@@ -8531,12 +8531,12 @@
         <v>100</v>
       </c>
       <c r="L96" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C97" s="12">
         <v>1</v>
@@ -8551,7 +8551,7 @@
         <v>176</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I97" s="19" t="s">
         <v>131</v>
@@ -8563,12 +8563,12 @@
         <v>100</v>
       </c>
       <c r="L97" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C98" s="11"/>
       <c r="D98" s="6">
@@ -8581,7 +8581,7 @@
         <v>184</v>
       </c>
       <c r="H98" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I98" s="19" t="s">
         <v>131</v>
@@ -8593,12 +8593,12 @@
         <v>100</v>
       </c>
       <c r="L98" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C99" s="11"/>
       <c r="D99" s="6">
@@ -8611,7 +8611,7 @@
         <v>179</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I99" s="19" t="s">
         <v>131</v>
@@ -8623,12 +8623,12 @@
         <v>100</v>
       </c>
       <c r="L99" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C100" s="11"/>
       <c r="D100" s="6">
@@ -8641,7 +8641,7 @@
         <v>130</v>
       </c>
       <c r="H100" s="17" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I100" s="19" t="s">
         <v>131</v>
@@ -8653,12 +8653,12 @@
         <v>100</v>
       </c>
       <c r="L100" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C101" s="11"/>
       <c r="D101" s="6">
@@ -8671,7 +8671,7 @@
         <v>177</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I101" s="19" t="s">
         <v>178</v>
@@ -8683,12 +8683,12 @@
         <v>100</v>
       </c>
       <c r="L101" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C102" s="11"/>
       <c r="D102" s="6">
@@ -8704,7 +8704,7 @@
         <v>132</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I102" s="19" t="s">
         <v>133</v>
@@ -8716,12 +8716,12 @@
         <v>100</v>
       </c>
       <c r="L102" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C103" s="11"/>
       <c r="D103" s="6">
@@ -8734,7 +8734,7 @@
         <v>137</v>
       </c>
       <c r="H103" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I103" s="19" t="s">
         <v>135</v>
@@ -8746,12 +8746,12 @@
         <v>100</v>
       </c>
       <c r="L103" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C104" s="11"/>
       <c r="D104" s="6">
@@ -8764,7 +8764,7 @@
         <v>134</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I104" s="19" t="s">
         <v>135</v>
@@ -8776,12 +8776,12 @@
         <v>100</v>
       </c>
       <c r="L104" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="16" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C105" s="11"/>
       <c r="D105" s="6">
@@ -8794,7 +8794,7 @@
         <v>136</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I105" s="19" t="s">
         <v>135</v>
@@ -8806,12 +8806,12 @@
         <v>100</v>
       </c>
       <c r="L105" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="16" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106" s="6">
@@ -8824,7 +8824,7 @@
         <v>138</v>
       </c>
       <c r="H106" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I106" s="19" t="s">
         <v>139</v>
@@ -8836,12 +8836,12 @@
         <v>100</v>
       </c>
       <c r="L106" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="107" spans="1:12">
       <c r="A107" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="6">
@@ -8857,7 +8857,7 @@
         <v>144</v>
       </c>
       <c r="H107" s="17" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I107" s="19" t="s">
         <v>143</v>
@@ -8869,12 +8869,12 @@
         <v>100</v>
       </c>
       <c r="L107" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="108" spans="1:12">
       <c r="A108" s="16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C108" s="11"/>
       <c r="D108" s="6">
@@ -8887,7 +8887,7 @@
         <v>140</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I108" s="19" t="s">
         <v>141</v>
@@ -8899,12 +8899,12 @@
         <v>100</v>
       </c>
       <c r="L108" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="109" spans="1:12">
       <c r="A109" s="16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C109" s="11"/>
       <c r="D109" s="6">
@@ -8917,7 +8917,7 @@
         <v>142</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I109" s="19" t="s">
         <v>143</v>
@@ -8929,12 +8929,12 @@
         <v>100</v>
       </c>
       <c r="L109" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="110" spans="1:12">
       <c r="A110" s="16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C110" s="10"/>
       <c r="D110" s="6">
@@ -8950,7 +8950,7 @@
         <v>145</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I110" s="19" t="s">
         <v>146</v>
@@ -8962,12 +8962,12 @@
         <v>100</v>
       </c>
       <c r="L110" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="111" spans="1:12">
       <c r="A111" s="16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C111" s="11"/>
       <c r="D111" s="6">
@@ -8980,7 +8980,7 @@
         <v>149</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I111" s="19" t="s">
         <v>150</v>
@@ -8992,12 +8992,12 @@
         <v>100</v>
       </c>
       <c r="L111" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="112" spans="1:12">
       <c r="A112" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C112" s="11"/>
       <c r="D112" s="6">
@@ -9010,7 +9010,7 @@
         <v>153</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I112" s="19" t="s">
         <v>152</v>
@@ -9022,12 +9022,12 @@
         <v>100</v>
       </c>
       <c r="L112" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="113" spans="1:12">
       <c r="A113" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C113" s="11"/>
       <c r="D113" s="6">
@@ -9040,7 +9040,7 @@
         <v>151</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I113" s="19" t="s">
         <v>152</v>
@@ -9052,12 +9052,12 @@
         <v>100</v>
       </c>
       <c r="L113" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="114" spans="1:12">
       <c r="A114" s="16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C114" s="11"/>
       <c r="E114" s="6">
@@ -9070,7 +9070,7 @@
         <v>171</v>
       </c>
       <c r="H114" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I114" s="19" t="s">
         <v>172</v>
@@ -9082,12 +9082,12 @@
         <v>100</v>
       </c>
       <c r="L114" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="115" spans="1:12">
       <c r="A115" s="16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C115" s="11"/>
       <c r="E115" s="6">
@@ -9100,7 +9100,7 @@
         <v>180</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I115" s="19" t="s">
         <v>181</v>
@@ -9112,12 +9112,12 @@
         <v>100</v>
       </c>
       <c r="L115" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="116" spans="1:12">
       <c r="A116" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C116" s="11"/>
       <c r="D116" s="6">
@@ -9133,7 +9133,7 @@
         <v>182</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I116" s="19" t="s">
         <v>183</v>
@@ -9145,7 +9145,7 @@
         <v>100</v>
       </c>
       <c r="L116" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -9166,7 +9166,7 @@
         <v>156</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I117" s="19" t="s">
         <v>157</v>
@@ -9178,12 +9178,12 @@
         <v>100</v>
       </c>
       <c r="L117" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="118" spans="1:12">
       <c r="A118" s="16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C118" s="11"/>
       <c r="D118" s="6">
@@ -9196,7 +9196,7 @@
         <v>161</v>
       </c>
       <c r="H118" s="17" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I118" s="19" t="s">
         <v>157</v>
@@ -9208,12 +9208,12 @@
         <v>100</v>
       </c>
       <c r="L118" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="119" spans="1:12">
       <c r="A119" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C119" s="12">
         <v>1</v>
@@ -9231,7 +9231,7 @@
         <v>158</v>
       </c>
       <c r="H119" s="17" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I119" s="19" t="s">
         <v>157</v>
@@ -9243,12 +9243,12 @@
         <v>100</v>
       </c>
       <c r="L119" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="120" spans="1:12">
       <c r="A120" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C120" s="11"/>
       <c r="D120" s="6">
@@ -9261,7 +9261,7 @@
         <v>159</v>
       </c>
       <c r="H120" s="17" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I120" s="19" t="s">
         <v>157</v>
@@ -9273,12 +9273,12 @@
         <v>100</v>
       </c>
       <c r="L120" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="121" spans="1:12">
       <c r="A121" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C121" s="11"/>
       <c r="D121" s="6">
@@ -9291,7 +9291,7 @@
         <v>160</v>
       </c>
       <c r="H121" s="17" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I121" s="19" t="s">
         <v>157</v>
@@ -9303,7 +9303,7 @@
         <v>100</v>
       </c>
       <c r="L121" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -9323,7 +9323,7 @@
         <v>128</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I122" s="19" t="s">
         <v>129</v>
@@ -9335,7 +9335,7 @@
         <v>100</v>
       </c>
       <c r="L122" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -9358,7 +9358,7 @@
         <v>185</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I123" s="19" t="s">
         <v>186</v>
@@ -9370,7 +9370,7 @@
         <v>100</v>
       </c>
       <c r="L123" s="23" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="124" spans="1:12">
@@ -9387,7 +9387,7 @@
         <v>187</v>
       </c>
       <c r="H124" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I124" s="19" t="s">
         <v>188</v>
@@ -9399,12 +9399,12 @@
         <v>100</v>
       </c>
       <c r="L124" s="23" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C125" s="12">
         <v>3</v>
@@ -9416,7 +9416,7 @@
         <v>189</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I125" s="19" t="s">
         <v>190</v>
@@ -9428,12 +9428,12 @@
         <v>100</v>
       </c>
       <c r="L125" s="23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C126" s="12">
         <v>1</v>
@@ -9445,7 +9445,7 @@
         <v>191</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I126" s="19" t="s">
         <v>192</v>
@@ -9457,24 +9457,24 @@
         <v>100</v>
       </c>
       <c r="L126" s="23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="16" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C127" s="12">
         <v>2</v>
       </c>
       <c r="F127" s="16" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G127" s="16" t="s">
         <v>193</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I127" s="19" t="s">
         <v>194</v>
@@ -9486,7 +9486,7 @@
         <v>100</v>
       </c>
       <c r="L127" s="23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="128" spans="1:12">
@@ -9507,7 +9507,7 @@
         <v>197</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I128" s="19" t="s">
         <v>196</v>
@@ -9519,12 +9519,12 @@
         <v>100</v>
       </c>
       <c r="L128" s="23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="129" spans="1:12">
       <c r="A129" s="16" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C129" s="11"/>
       <c r="E129" s="6">
@@ -9537,7 +9537,7 @@
         <v>198</v>
       </c>
       <c r="H129" s="17" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I129" s="19" t="s">
         <v>196</v>
@@ -9549,12 +9549,12 @@
         <v>100</v>
       </c>
       <c r="L129" s="23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="130" spans="1:12">
       <c r="A130" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C130" s="11"/>
       <c r="E130" s="6">
@@ -9567,7 +9567,7 @@
         <v>195</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I130" s="19" t="s">
         <v>196</v>
@@ -9579,7 +9579,7 @@
         <v>100</v>
       </c>
       <c r="L130" s="23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="131" spans="1:12">
@@ -9602,7 +9602,7 @@
         <v>199</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I131" s="19" t="s">
         <v>200</v>
@@ -9614,12 +9614,12 @@
         <v>100</v>
       </c>
       <c r="L131" s="23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="132" spans="1:12">
       <c r="A132" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C132" s="12">
         <v>1</v>
@@ -9631,7 +9631,7 @@
         <v>201</v>
       </c>
       <c r="H132" s="17" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I132" s="19" t="s">
         <v>202</v>
@@ -9643,7 +9643,7 @@
         <v>100</v>
       </c>
       <c r="L132" s="23" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -9661,7 +9661,7 @@
         <v>203</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I133" s="19" t="s">
         <v>204</v>
@@ -9673,24 +9673,24 @@
         <v>100</v>
       </c>
       <c r="L133" s="23" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="134" spans="1:12">
       <c r="A134" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="C134" s="12">
+        <v>1</v>
+      </c>
+      <c r="F134" s="16" t="s">
         <v>563</v>
-      </c>
-      <c r="C134" s="12">
-        <v>1</v>
-      </c>
-      <c r="F134" s="16" t="s">
-        <v>564</v>
       </c>
       <c r="G134" s="16" t="s">
         <v>205</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I134" s="19" t="s">
         <v>206</v>
@@ -9702,12 +9702,12 @@
         <v>100</v>
       </c>
       <c r="L134" s="23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="135" spans="1:12">
       <c r="A135" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C135" s="12">
         <v>2</v>
@@ -9719,7 +9719,7 @@
         <v>207</v>
       </c>
       <c r="H135" s="17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I135" s="19" t="s">
         <v>208</v>
@@ -9731,12 +9731,12 @@
         <v>100</v>
       </c>
       <c r="L135" s="23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="136" spans="1:12">
       <c r="A136" s="20" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C136" s="11"/>
       <c r="D136" s="6">
@@ -9752,7 +9752,7 @@
         <v>209</v>
       </c>
       <c r="H136" s="17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I136" s="19" t="s">
         <v>210</v>
@@ -9764,7 +9764,7 @@
         <v>99</v>
       </c>
       <c r="L136" s="23" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -9781,7 +9781,7 @@
         <v>211</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I137" s="19" t="s">
         <v>212</v>
@@ -9793,12 +9793,12 @@
         <v>100</v>
       </c>
       <c r="L137" s="23" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="138" spans="1:12">
       <c r="A138" s="16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B138" s="6">
         <v>1</v>
@@ -9811,7 +9811,7 @@
         <v>213</v>
       </c>
       <c r="H138" s="17" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I138" s="19" t="s">
         <v>214</v>
@@ -9823,7 +9823,7 @@
         <v>100</v>
       </c>
       <c r="L138" s="23" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -9841,7 +9841,7 @@
         <v>215</v>
       </c>
       <c r="H139" s="17" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I139" s="19" t="s">
         <v>216</v>
@@ -9853,12 +9853,12 @@
         <v>100</v>
       </c>
       <c r="L139" s="23" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="140" spans="1:12">
       <c r="A140" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B140" s="17">
         <v>29</v>

</xml_diff>